<commit_message>
TraceGenerator upgraded to SimpleTemplates
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_simple_de.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_simple_de.xlsx
@@ -1160,6 +1160,30 @@
     <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="33" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1197,12 +1221,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="35" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1210,24 +1228,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="30" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1646,7 +1646,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
@@ -1688,60 +1688,60 @@
     </row>
     <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:13" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="39" t="s">
+      <c r="A3" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
-      <c r="G3" s="40"/>
-      <c r="H3" s="40"/>
-      <c r="I3" s="40"/>
-      <c r="J3" s="40"/>
-      <c r="K3" s="40"/>
-      <c r="L3" s="40"/>
+      <c r="B3" s="48"/>
+      <c r="C3" s="48"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="48"/>
+      <c r="F3" s="48"/>
+      <c r="G3" s="48"/>
+      <c r="H3" s="48"/>
+      <c r="I3" s="48"/>
+      <c r="J3" s="48"/>
+      <c r="K3" s="48"/>
+      <c r="L3" s="48"/>
     </row>
     <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="49" t="s">
+      <c r="A4" s="57" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="56" t="s">
+      <c r="F4" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="51" t="s">
+      <c r="G4" s="40"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="37" t="s">
         <v>20</v>
       </c>
-      <c r="J4" s="58" t="s">
+      <c r="J4" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="K4" s="59"/>
-      <c r="L4" s="37" t="s">
+      <c r="K4" s="42"/>
+      <c r="L4" s="45" t="s">
         <v>15</v>
       </c>
       <c r="M4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="27.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="50"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="52"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="A5" s="58"/>
+      <c r="B5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="38"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="29" t="s">
         <v>0</v>
       </c>
@@ -1751,14 +1751,14 @@
       <c r="H5" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="I5" s="52"/>
+      <c r="I5" s="38"/>
       <c r="J5" s="34" t="s">
         <v>27</v>
       </c>
       <c r="K5" s="34" t="s">
         <v>28</v>
       </c>
-      <c r="L5" s="38"/>
+      <c r="L5" s="46"/>
     </row>
     <row r="6" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="14" t="s">
@@ -1876,59 +1876,59 @@
       <c r="K13" s="20"/>
     </row>
     <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="43"/>
+      <c r="B14" s="50"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="50"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="50"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="50"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="50"/>
+      <c r="L14" s="51"/>
     </row>
     <row r="15" spans="1:13" s="21" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="55" t="s">
         <v>33</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="52" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="44" t="s">
+      <c r="C15" s="52" t="s">
         <v>10</v>
       </c>
-      <c r="D15" s="44" t="s">
+      <c r="D15" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="54" t="s">
+      <c r="F15" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="44" t="s">
+      <c r="G15" s="61"/>
+      <c r="H15" s="61"/>
+      <c r="I15" s="52" t="s">
         <v>21</v>
       </c>
-      <c r="J15" s="60" t="s">
+      <c r="J15" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="61"/>
-      <c r="L15" s="37" t="s">
+      <c r="K15" s="44"/>
+      <c r="L15" s="45" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="21" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="48"/>
-      <c r="B16" s="46"/>
-      <c r="C16" s="46"/>
-      <c r="D16" s="45"/>
-      <c r="E16" s="53"/>
+      <c r="A16" s="56"/>
+      <c r="B16" s="54"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="59"/>
       <c r="F16" s="35" t="s">
         <v>0</v>
       </c>
@@ -1938,14 +1938,14 @@
       <c r="H16" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="53"/>
+      <c r="I16" s="59"/>
       <c r="J16" s="35" t="s">
         <v>27</v>
       </c>
       <c r="K16" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="L16" s="38"/>
+      <c r="L16" s="46"/>
     </row>
     <row r="17" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
@@ -3156,11 +3156,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L4:L5"/>
     <mergeCell ref="A3:L3"/>
     <mergeCell ref="A14:L14"/>
     <mergeCell ref="L15:L16"/>
@@ -3176,6 +3171,11 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:H15"/>
     <mergeCell ref="I15:I16"/>
+    <mergeCell ref="I4:I5"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="L4:L5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Simple Templates final spec definition
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_simple_de.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_simple_de.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="35">
   <si>
     <t>Tag</t>
   </si>
@@ -31,31 +31,10 @@
     <t>Chargennummer</t>
   </si>
   <si>
-    <t>Produktname</t>
-  </si>
-  <si>
     <t>EAN</t>
   </si>
   <si>
     <t>Für Rückfragen bitte einfach anrufen: Dr. Armin Weiser, 030 - 18412-2118, armin.weiser@bfr.bund.de</t>
-  </si>
-  <si>
-    <t>Zutat - Produktname</t>
-  </si>
-  <si>
-    <t>Zutat - Chargennummer</t>
-  </si>
-  <si>
-    <t>Zutat - EAN</t>
-  </si>
-  <si>
-    <t>Wareneingang - chargenbasierte Zutatenliste</t>
-  </si>
-  <si>
-    <t>Zutat - Wareneingang</t>
-  </si>
-  <si>
-    <t>Ankunftsdatum Empfänger</t>
   </si>
   <si>
     <t>anzufragender
@@ -68,23 +47,10 @@
     <t>MHD oder Verbrauchsdatum</t>
   </si>
   <si>
-    <t>Zutat - MHD oder Verbrauchsdatum</t>
-  </si>
-  <si>
     <t>Digitale Auszüge (z.B. Excel oder xml-Dateien) vom befragten Betrieb könnten ebenso geeignet sein; das Ausfüllen dieser Vorlage wäre dann nicht notwendig - für diesen Fall bitte Rückruf (Dr. Armin Weiser: 030 - 18412-2118)</t>
   </si>
   <si>
     <t>Die Warenausgänge sind bekannt (siehe oben, graue Felder)</t>
-  </si>
-  <si>
-    <t>abgegebene
-Menge
-(z.B. 4 Kartons a 10kg)</t>
-  </si>
-  <si>
-    <t>Zutat -
-empfangene Menge
-(z.B. 4 Kartons a 10kg)</t>
   </si>
   <si>
     <t>Company</t>
@@ -126,12 +92,56 @@
   <si>
     <t xml:space="preserve"> </t>
   </si>
+  <si>
+    <t>Bezeichnung</t>
+  </si>
+  <si>
+    <t>Zutat</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>Lieferung</t>
+  </si>
+  <si>
+    <t>Produkt</t>
+  </si>
+  <si>
+    <t>abgegebene Menge
+(z.B. 4 Kartons a 10kg)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Wareneingang - chargenbasierte </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="16"/>
+        <color theme="0"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Zutatenliste</t>
+    </r>
+  </si>
+  <si>
+    <t>Lotinformation</t>
+  </si>
+  <si>
+    <t>Lieferdatum</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="37" x14ac:knownFonts="1">
+  <fonts count="38" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -390,6 +400,14 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -569,7 +587,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -741,19 +759,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -926,15 +931,79 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
-        <color indexed="64"/>
+      <right style="thin">
+        <color auto="1"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1052,27 +1121,27 @@
     <xf numFmtId="0" fontId="27" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="32" fillId="29" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="32" fillId="29" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="5" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1081,13 +1150,10 @@
     <xf numFmtId="49" fontId="7" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
@@ -1103,10 +1169,10 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="4" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
@@ -1119,13 +1185,13 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
@@ -1135,7 +1201,7 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1145,89 +1211,120 @@
     <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="7" fillId="5" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="1" fontId="7" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="6" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="1" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="30" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="30" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="30" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1644,1538 +1741,1701 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:N105"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.3984375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.73046875" style="10" customWidth="1"/>
-    <col min="2" max="2" width="25.86328125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="12.46484375" style="10" customWidth="1"/>
-    <col min="4" max="4" width="16" style="10" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" style="10" customWidth="1"/>
-    <col min="6" max="6" width="7.33203125" style="27" customWidth="1"/>
-    <col min="7" max="7" width="7.73046875" style="27" customWidth="1"/>
-    <col min="8" max="8" width="9.19921875" style="27" customWidth="1"/>
-    <col min="9" max="9" width="22.06640625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="21.265625" style="10" customWidth="1"/>
-    <col min="11" max="11" width="39.9296875" style="10" customWidth="1"/>
-    <col min="12" max="12" width="19.33203125" style="10" customWidth="1"/>
-    <col min="13" max="13" width="26.9296875" style="10" customWidth="1"/>
-    <col min="14" max="16384" width="11.3984375" style="10"/>
+    <col min="1" max="1" width="19.73046875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.86328125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="12.46484375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="16" style="9" customWidth="1"/>
+    <col min="5" max="5" width="16.33203125" style="9" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="7.73046875" style="26" customWidth="1"/>
+    <col min="8" max="8" width="9.19921875" style="26" customWidth="1"/>
+    <col min="9" max="9" width="22.06640625" style="9" customWidth="1"/>
+    <col min="10" max="10" width="21.265625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="39.9296875" style="9" customWidth="1"/>
+    <col min="12" max="12" width="10.53125" style="9" customWidth="1"/>
+    <col min="13" max="13" width="19.33203125" style="9" customWidth="1"/>
+    <col min="14" max="14" width="26.9296875" style="9" customWidth="1"/>
+    <col min="15" max="16384" width="11.3984375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:14" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="8"/>
+      <c r="F1" s="25"/>
+      <c r="H1" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+    </row>
+    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:14" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="59"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="59"/>
+    </row>
+    <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="41" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="51"/>
+      <c r="D4" s="50" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="51"/>
+      <c r="F4" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="46" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="47"/>
+      <c r="L4" s="47"/>
+      <c r="M4" s="43" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="12"/>
+    </row>
+    <row r="5" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="39"/>
+      <c r="B5" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="J5" s="65" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="65" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="M5" s="44"/>
+      <c r="N5" s="12"/>
+    </row>
+    <row r="6" spans="1:14" ht="12.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="42"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>1</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="64"/>
+      <c r="J6" s="57"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
+      <c r="M6" s="45"/>
+    </row>
+    <row r="7" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="16"/>
+      <c r="L7" s="16"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="9"/>
+    </row>
+    <row r="8" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="19"/>
+      <c r="L8" s="19"/>
+    </row>
+    <row r="9" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="J9" s="19"/>
+      <c r="K9" s="19"/>
+      <c r="L9" s="19"/>
+    </row>
+    <row r="10" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+    </row>
+    <row r="11" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A11" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" s="19"/>
+      <c r="C11" s="19"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+    </row>
+    <row r="12" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="J12" s="19"/>
+      <c r="K12" s="19"/>
+      <c r="L12" s="19"/>
+    </row>
+    <row r="13" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D1" s="8"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="26"/>
-      <c r="H1" s="28" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-    </row>
-    <row r="2" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:13" s="12" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="47" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="48"/>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="48"/>
-      <c r="K3" s="48"/>
-      <c r="L3" s="48"/>
-    </row>
-    <row r="4" spans="1:13" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="57" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="40"/>
-      <c r="H4" s="40"/>
-      <c r="I4" s="37" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="41" t="s">
-        <v>26</v>
-      </c>
-      <c r="K4" s="42"/>
-      <c r="L4" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="M4" s="13"/>
-    </row>
-    <row r="5" spans="1:13" ht="27.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="58"/>
-      <c r="B5" s="38"/>
-      <c r="C5" s="38"/>
-      <c r="D5" s="38"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="29" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="29" t="s">
-        <v>1</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>2</v>
-      </c>
-      <c r="I5" s="38"/>
-      <c r="J5" s="34" t="s">
-        <v>27</v>
-      </c>
-      <c r="K5" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="L5" s="46"/>
-    </row>
-    <row r="6" spans="1:13" s="12" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="17"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="10"/>
-    </row>
-    <row r="7" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="36" t="s">
-        <v>30</v>
-      </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="31"/>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-    </row>
-    <row r="8" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="20"/>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="31"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="31"/>
-      <c r="J8" s="20"/>
-      <c r="K8" s="20"/>
-    </row>
-    <row r="9" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="20"/>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="31"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="J9" s="20"/>
-      <c r="K9" s="20"/>
-    </row>
-    <row r="10" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-    </row>
-    <row r="11" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B11" s="20"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="31"/>
-      <c r="G11" s="31"/>
-      <c r="H11" s="31"/>
-      <c r="J11" s="20"/>
-      <c r="K11" s="20"/>
-    </row>
-    <row r="12" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="19" t="s">
+      <c r="B13" s="19"/>
+      <c r="C13" s="19"/>
+      <c r="D13" s="19"/>
+      <c r="E13" s="19"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="J13" s="19"/>
+      <c r="K13" s="19"/>
+      <c r="L13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="19"/>
+      <c r="E14" s="19"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="J14" s="19"/>
+      <c r="K14" s="19"/>
+      <c r="L14" s="19"/>
+    </row>
+    <row r="15" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="31"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="31"/>
-      <c r="J12" s="20"/>
-      <c r="K12" s="20"/>
-    </row>
-    <row r="13" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
-      <c r="H13" s="31"/>
-      <c r="J13" s="20"/>
-      <c r="K13" s="20"/>
-    </row>
-    <row r="14" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="49" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
-      <c r="E14" s="50"/>
-      <c r="F14" s="50"/>
-      <c r="G14" s="50"/>
-      <c r="H14" s="50"/>
-      <c r="I14" s="50"/>
-      <c r="J14" s="50"/>
-      <c r="K14" s="50"/>
-      <c r="L14" s="51"/>
-    </row>
-    <row r="15" spans="1:13" s="21" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="55" t="s">
-        <v>33</v>
-      </c>
-      <c r="B15" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="52" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" s="52" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="52" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="60" t="s">
-        <v>12</v>
-      </c>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="61"/>
+      <c r="E15" s="61"/>
+      <c r="F15" s="61"/>
       <c r="G15" s="61"/>
       <c r="H15" s="61"/>
-      <c r="I15" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="J15" s="43" t="s">
+      <c r="I15" s="61"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="61"/>
+      <c r="L15" s="61"/>
+      <c r="M15" s="62"/>
+    </row>
+    <row r="16" spans="1:14" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="52" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="51"/>
+      <c r="F16" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="K15" s="44"/>
-      <c r="L15" s="45" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" s="21" customFormat="1" ht="37.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="56"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="54"/>
-      <c r="D16" s="53"/>
-      <c r="E16" s="59"/>
-      <c r="F16" s="35" t="s">
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="K16" s="49"/>
+      <c r="L16" s="47"/>
+      <c r="M16" s="36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="20" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17" s="39"/>
+      <c r="B17" s="56" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="67" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="68"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="66" t="s">
+        <v>17</v>
+      </c>
+      <c r="K17" s="66" t="s">
+        <v>18</v>
+      </c>
+      <c r="L17" s="66" t="s">
+        <v>27</v>
+      </c>
+      <c r="M17" s="37"/>
+    </row>
+    <row r="18" spans="1:13" s="20" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18" s="40"/>
+      <c r="B18" s="57"/>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="G16" s="35" t="s">
+      <c r="G18" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H16" s="35" t="s">
+      <c r="H18" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I16" s="59"/>
-      <c r="J16" s="35" t="s">
-        <v>27</v>
-      </c>
-      <c r="K16" s="35" t="s">
-        <v>28</v>
-      </c>
-      <c r="L16" s="46"/>
-    </row>
-    <row r="17" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="18"/>
-    </row>
-    <row r="18" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="3"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="32"/>
-      <c r="H18" s="32"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="18"/>
-      <c r="K18" s="22"/>
-      <c r="L18" s="18"/>
-    </row>
-    <row r="19" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="I18" s="57"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="38"/>
+    </row>
+    <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="1"/>
       <c r="C19" s="2"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="32"/>
-      <c r="H19" s="32"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
+      <c r="H19" s="31"/>
       <c r="I19" s="1"/>
-      <c r="J19" s="18"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="18"/>
-    </row>
-    <row r="20" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J19" s="1"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="17"/>
+    </row>
+    <row r="20" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="1"/>
       <c r="C20" s="2"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="32"/>
-      <c r="H20" s="32"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
+      <c r="H20" s="31"/>
       <c r="I20" s="1"/>
-      <c r="J20" s="18"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="18"/>
-    </row>
-    <row r="21" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J20" s="17"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="17"/>
+    </row>
+    <row r="21" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="1"/>
       <c r="C21" s="2"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="18"/>
-      <c r="K21" s="22"/>
-      <c r="L21" s="18"/>
-    </row>
-    <row r="22" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J21" s="17"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="17"/>
+    </row>
+    <row r="22" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="1"/>
       <c r="C22" s="2"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="32"/>
-      <c r="H22" s="32"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
+      <c r="H22" s="31"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="22"/>
-      <c r="L22" s="18"/>
-    </row>
-    <row r="23" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J22" s="17"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="17"/>
+    </row>
+    <row r="23" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="1"/>
       <c r="C23" s="2"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="32"/>
-      <c r="H23" s="32"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="22"/>
-      <c r="L23" s="18"/>
-    </row>
-    <row r="24" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J23" s="17"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="17"/>
+    </row>
+    <row r="24" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
+      <c r="C24" s="2"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="32"/>
-      <c r="H24" s="32"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="22"/>
-      <c r="L24" s="18"/>
-    </row>
-    <row r="25" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J24" s="17"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="17"/>
+    </row>
+    <row r="25" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
+      <c r="C25" s="2"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="32"/>
-      <c r="G25" s="32"/>
-      <c r="H25" s="32"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
+      <c r="H25" s="31"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="22"/>
-      <c r="L25" s="18"/>
-    </row>
-    <row r="26" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J25" s="17"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="17"/>
+    </row>
+    <row r="26" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="32"/>
-      <c r="H26" s="32"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
+      <c r="H26" s="31"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="22"/>
-      <c r="L26" s="18"/>
-    </row>
-    <row r="27" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J26" s="17"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="17"/>
+    </row>
+    <row r="27" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="32"/>
-      <c r="G27" s="32"/>
-      <c r="H27" s="32"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="18"/>
-      <c r="K27" s="22"/>
-      <c r="L27" s="18"/>
-    </row>
-    <row r="28" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J27" s="17"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="17"/>
+    </row>
+    <row r="28" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="32"/>
-      <c r="H28" s="32"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
+      <c r="H28" s="31"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="18"/>
-      <c r="K28" s="22"/>
-      <c r="L28" s="18"/>
-    </row>
-    <row r="29" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J28" s="17"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="17"/>
+    </row>
+    <row r="29" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="32"/>
-      <c r="G29" s="32"/>
-      <c r="H29" s="32"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="18"/>
-      <c r="K29" s="22"/>
-      <c r="L29" s="18"/>
-    </row>
-    <row r="30" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J29" s="17"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="17"/>
+    </row>
+    <row r="30" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="32"/>
-      <c r="H30" s="32"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
+      <c r="H30" s="31"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="18"/>
-      <c r="K30" s="22"/>
-      <c r="L30" s="18"/>
-    </row>
-    <row r="31" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J30" s="17"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="17"/>
+    </row>
+    <row r="31" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="32"/>
-      <c r="H31" s="32"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="18"/>
-      <c r="K31" s="22"/>
-      <c r="L31" s="18"/>
-    </row>
-    <row r="32" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J31" s="17"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="17"/>
+    </row>
+    <row r="32" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="32"/>
-      <c r="G32" s="32"/>
-      <c r="H32" s="32"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="18"/>
-      <c r="K32" s="22"/>
-      <c r="L32" s="18"/>
-    </row>
-    <row r="33" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J32" s="17"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="17"/>
+    </row>
+    <row r="33" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="32"/>
-      <c r="H33" s="32"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="31"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="18"/>
-      <c r="K33" s="22"/>
-      <c r="L33" s="18"/>
-    </row>
-    <row r="34" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J33" s="17"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="17"/>
+    </row>
+    <row r="34" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="32"/>
-      <c r="G34" s="32"/>
-      <c r="H34" s="32"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
+      <c r="H34" s="31"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="18"/>
-      <c r="K34" s="22"/>
-      <c r="L34" s="18"/>
-    </row>
-    <row r="35" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J34" s="17"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="17"/>
+    </row>
+    <row r="35" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
+      <c r="H35" s="31"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="18"/>
-    </row>
-    <row r="36" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J35" s="17"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="17"/>
+    </row>
+    <row r="36" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="32"/>
-      <c r="H36" s="32"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
+      <c r="H36" s="31"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="22"/>
-      <c r="L36" s="18"/>
-    </row>
-    <row r="37" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J36" s="17"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="17"/>
+    </row>
+    <row r="37" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="32"/>
-      <c r="G37" s="32"/>
-      <c r="H37" s="32"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="22"/>
-      <c r="L37" s="18"/>
-    </row>
-    <row r="38" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J37" s="17"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="17"/>
+    </row>
+    <row r="38" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-      <c r="F38" s="32"/>
-      <c r="G38" s="32"/>
-      <c r="H38" s="32"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
+      <c r="H38" s="31"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="18"/>
-      <c r="K38" s="22"/>
-      <c r="L38" s="18"/>
-    </row>
-    <row r="39" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J38" s="17"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="17"/>
+    </row>
+    <row r="39" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="32"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
+      <c r="H39" s="31"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="18"/>
-      <c r="K39" s="22"/>
-      <c r="L39" s="18"/>
-    </row>
-    <row r="40" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J39" s="17"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="17"/>
+    </row>
+    <row r="40" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="32"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
+      <c r="H40" s="31"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="18"/>
-      <c r="K40" s="22"/>
-      <c r="L40" s="18"/>
-    </row>
-    <row r="41" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J40" s="17"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="17"/>
+    </row>
+    <row r="41" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="32"/>
+      <c r="F41" s="31"/>
+      <c r="G41" s="31"/>
+      <c r="H41" s="31"/>
       <c r="I41" s="1"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="22"/>
-      <c r="L41" s="18"/>
-    </row>
-    <row r="42" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J41" s="17"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="17"/>
+    </row>
+    <row r="42" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="32"/>
+      <c r="F42" s="31"/>
+      <c r="G42" s="31"/>
+      <c r="H42" s="31"/>
       <c r="I42" s="1"/>
-      <c r="J42" s="18"/>
-      <c r="K42" s="22"/>
-      <c r="L42" s="18"/>
-    </row>
-    <row r="43" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J42" s="17"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="17"/>
+    </row>
+    <row r="43" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="32"/>
+      <c r="F43" s="31"/>
+      <c r="G43" s="31"/>
+      <c r="H43" s="31"/>
       <c r="I43" s="1"/>
-      <c r="J43" s="18"/>
-      <c r="K43" s="22"/>
-      <c r="L43" s="18"/>
-    </row>
-    <row r="44" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J43" s="17"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="17"/>
+    </row>
+    <row r="44" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="32"/>
+      <c r="F44" s="31"/>
+      <c r="G44" s="31"/>
+      <c r="H44" s="31"/>
       <c r="I44" s="1"/>
-      <c r="J44" s="18"/>
-      <c r="K44" s="22"/>
-      <c r="L44" s="18"/>
-    </row>
-    <row r="45" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J44" s="17"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="17"/>
+    </row>
+    <row r="45" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="32"/>
-      <c r="H45" s="32"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="31"/>
+      <c r="H45" s="31"/>
       <c r="I45" s="1"/>
-      <c r="J45" s="18"/>
-      <c r="K45" s="22"/>
-      <c r="L45" s="18"/>
-    </row>
-    <row r="46" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J45" s="17"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="17"/>
+    </row>
+    <row r="46" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
-      <c r="H46" s="32"/>
+      <c r="F46" s="31"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
       <c r="I46" s="1"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="18"/>
-    </row>
-    <row r="47" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J46" s="17"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="17"/>
+    </row>
+    <row r="47" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
-      <c r="H47" s="32"/>
+      <c r="F47" s="31"/>
+      <c r="G47" s="31"/>
+      <c r="H47" s="31"/>
       <c r="I47" s="1"/>
-      <c r="J47" s="18"/>
-      <c r="K47" s="22"/>
-      <c r="L47" s="18"/>
-    </row>
-    <row r="48" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J47" s="17"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21"/>
+      <c r="M47" s="17"/>
+    </row>
+    <row r="48" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
-      <c r="H48" s="32"/>
+      <c r="F48" s="31"/>
+      <c r="G48" s="31"/>
+      <c r="H48" s="31"/>
       <c r="I48" s="1"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="22"/>
-      <c r="L48" s="18"/>
-    </row>
-    <row r="49" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J48" s="17"/>
+      <c r="K48" s="21"/>
+      <c r="L48" s="21"/>
+      <c r="M48" s="17"/>
+    </row>
+    <row r="49" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="32"/>
-      <c r="G49" s="32"/>
-      <c r="H49" s="32"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="31"/>
+      <c r="H49" s="31"/>
       <c r="I49" s="1"/>
-      <c r="J49" s="18"/>
-      <c r="K49" s="22"/>
-      <c r="L49" s="18"/>
-    </row>
-    <row r="50" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J49" s="17"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21"/>
+      <c r="M49" s="17"/>
+    </row>
+    <row r="50" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="32"/>
-      <c r="G50" s="32"/>
-      <c r="H50" s="32"/>
+      <c r="F50" s="31"/>
+      <c r="G50" s="31"/>
+      <c r="H50" s="31"/>
       <c r="I50" s="1"/>
-      <c r="J50" s="18"/>
-      <c r="K50" s="22"/>
-      <c r="L50" s="18"/>
-    </row>
-    <row r="51" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J50" s="17"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21"/>
+      <c r="M50" s="17"/>
+    </row>
+    <row r="51" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="32"/>
-      <c r="H51" s="32"/>
+      <c r="F51" s="31"/>
+      <c r="G51" s="31"/>
+      <c r="H51" s="31"/>
       <c r="I51" s="1"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="22"/>
-      <c r="L51" s="18"/>
-    </row>
-    <row r="52" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J51" s="17"/>
+      <c r="K51" s="21"/>
+      <c r="L51" s="21"/>
+      <c r="M51" s="17"/>
+    </row>
+    <row r="52" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="32"/>
-      <c r="G52" s="32"/>
-      <c r="H52" s="32"/>
+      <c r="F52" s="31"/>
+      <c r="G52" s="31"/>
+      <c r="H52" s="31"/>
       <c r="I52" s="1"/>
-      <c r="J52" s="18"/>
-      <c r="K52" s="22"/>
-      <c r="L52" s="18"/>
-    </row>
-    <row r="53" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J52" s="17"/>
+      <c r="K52" s="21"/>
+      <c r="L52" s="21"/>
+      <c r="M52" s="17"/>
+    </row>
+    <row r="53" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="32"/>
-      <c r="G53" s="32"/>
-      <c r="H53" s="32"/>
+      <c r="F53" s="31"/>
+      <c r="G53" s="31"/>
+      <c r="H53" s="31"/>
       <c r="I53" s="1"/>
-      <c r="J53" s="18"/>
-      <c r="K53" s="22"/>
-      <c r="L53" s="18"/>
-    </row>
-    <row r="54" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J53" s="17"/>
+      <c r="K53" s="21"/>
+      <c r="L53" s="21"/>
+      <c r="M53" s="17"/>
+    </row>
+    <row r="54" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="32"/>
-      <c r="G54" s="32"/>
-      <c r="H54" s="32"/>
+      <c r="F54" s="31"/>
+      <c r="G54" s="31"/>
+      <c r="H54" s="31"/>
       <c r="I54" s="1"/>
-      <c r="J54" s="18"/>
-      <c r="K54" s="22"/>
-      <c r="L54" s="18"/>
-    </row>
-    <row r="55" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J54" s="17"/>
+      <c r="K54" s="21"/>
+      <c r="L54" s="21"/>
+      <c r="M54" s="17"/>
+    </row>
+    <row r="55" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
-      <c r="F55" s="32"/>
-      <c r="G55" s="32"/>
-      <c r="H55" s="32"/>
+      <c r="F55" s="31"/>
+      <c r="G55" s="31"/>
+      <c r="H55" s="31"/>
       <c r="I55" s="1"/>
-      <c r="J55" s="18"/>
-      <c r="K55" s="22"/>
-      <c r="L55" s="18"/>
-    </row>
-    <row r="56" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J55" s="17"/>
+      <c r="K55" s="21"/>
+      <c r="L55" s="21"/>
+      <c r="M55" s="17"/>
+    </row>
+    <row r="56" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="32"/>
-      <c r="G56" s="32"/>
-      <c r="H56" s="32"/>
+      <c r="F56" s="31"/>
+      <c r="G56" s="31"/>
+      <c r="H56" s="31"/>
       <c r="I56" s="1"/>
-      <c r="J56" s="18"/>
-      <c r="K56" s="22"/>
-      <c r="L56" s="18"/>
-    </row>
-    <row r="57" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J56" s="17"/>
+      <c r="K56" s="21"/>
+      <c r="L56" s="21"/>
+      <c r="M56" s="17"/>
+    </row>
+    <row r="57" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="32"/>
-      <c r="G57" s="32"/>
-      <c r="H57" s="32"/>
+      <c r="F57" s="31"/>
+      <c r="G57" s="31"/>
+      <c r="H57" s="31"/>
       <c r="I57" s="1"/>
-      <c r="J57" s="18"/>
-      <c r="K57" s="22"/>
-      <c r="L57" s="18"/>
-    </row>
-    <row r="58" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J57" s="17"/>
+      <c r="K57" s="21"/>
+      <c r="L57" s="21"/>
+      <c r="M57" s="17"/>
+    </row>
+    <row r="58" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="32"/>
-      <c r="G58" s="32"/>
-      <c r="H58" s="32"/>
+      <c r="F58" s="31"/>
+      <c r="G58" s="31"/>
+      <c r="H58" s="31"/>
       <c r="I58" s="1"/>
-      <c r="J58" s="18"/>
-      <c r="K58" s="22"/>
-      <c r="L58" s="18"/>
-    </row>
-    <row r="59" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J58" s="17"/>
+      <c r="K58" s="21"/>
+      <c r="L58" s="21"/>
+      <c r="M58" s="17"/>
+    </row>
+    <row r="59" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="32"/>
-      <c r="G59" s="32"/>
-      <c r="H59" s="32"/>
+      <c r="F59" s="31"/>
+      <c r="G59" s="31"/>
+      <c r="H59" s="31"/>
       <c r="I59" s="1"/>
-      <c r="J59" s="18"/>
-      <c r="K59" s="22"/>
-      <c r="L59" s="18"/>
-    </row>
-    <row r="60" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J59" s="17"/>
+      <c r="K59" s="21"/>
+      <c r="L59" s="21"/>
+      <c r="M59" s="17"/>
+    </row>
+    <row r="60" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="32"/>
-      <c r="H60" s="32"/>
+      <c r="F60" s="31"/>
+      <c r="G60" s="31"/>
+      <c r="H60" s="31"/>
       <c r="I60" s="1"/>
-      <c r="J60" s="18"/>
-      <c r="K60" s="22"/>
-      <c r="L60" s="18"/>
-    </row>
-    <row r="61" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J60" s="17"/>
+      <c r="K60" s="21"/>
+      <c r="L60" s="21"/>
+      <c r="M60" s="17"/>
+    </row>
+    <row r="61" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="32"/>
-      <c r="G61" s="32"/>
-      <c r="H61" s="32"/>
+      <c r="F61" s="31"/>
+      <c r="G61" s="31"/>
+      <c r="H61" s="31"/>
       <c r="I61" s="1"/>
-      <c r="J61" s="18"/>
-      <c r="K61" s="22"/>
-      <c r="L61" s="18"/>
-    </row>
-    <row r="62" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J61" s="17"/>
+      <c r="K61" s="21"/>
+      <c r="L61" s="21"/>
+      <c r="M61" s="17"/>
+    </row>
+    <row r="62" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="32"/>
-      <c r="G62" s="32"/>
-      <c r="H62" s="32"/>
+      <c r="F62" s="31"/>
+      <c r="G62" s="31"/>
+      <c r="H62" s="31"/>
       <c r="I62" s="1"/>
-      <c r="J62" s="18"/>
-      <c r="K62" s="22"/>
-      <c r="L62" s="18"/>
-    </row>
-    <row r="63" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J62" s="17"/>
+      <c r="K62" s="21"/>
+      <c r="L62" s="21"/>
+      <c r="M62" s="17"/>
+    </row>
+    <row r="63" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="32"/>
-      <c r="G63" s="32"/>
-      <c r="H63" s="32"/>
+      <c r="F63" s="31"/>
+      <c r="G63" s="31"/>
+      <c r="H63" s="31"/>
       <c r="I63" s="1"/>
-      <c r="J63" s="18"/>
-      <c r="K63" s="22"/>
-      <c r="L63" s="18"/>
-    </row>
-    <row r="64" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J63" s="17"/>
+      <c r="K63" s="21"/>
+      <c r="L63" s="21"/>
+      <c r="M63" s="17"/>
+    </row>
+    <row r="64" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="32"/>
-      <c r="G64" s="32"/>
-      <c r="H64" s="32"/>
+      <c r="F64" s="31"/>
+      <c r="G64" s="31"/>
+      <c r="H64" s="31"/>
       <c r="I64" s="1"/>
-      <c r="J64" s="18"/>
-      <c r="K64" s="22"/>
-      <c r="L64" s="18"/>
-    </row>
-    <row r="65" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J64" s="17"/>
+      <c r="K64" s="21"/>
+      <c r="L64" s="21"/>
+      <c r="M64" s="17"/>
+    </row>
+    <row r="65" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
-      <c r="F65" s="32"/>
-      <c r="G65" s="32"/>
-      <c r="H65" s="32"/>
+      <c r="F65" s="31"/>
+      <c r="G65" s="31"/>
+      <c r="H65" s="31"/>
       <c r="I65" s="1"/>
-      <c r="J65" s="18"/>
-      <c r="K65" s="22"/>
-      <c r="L65" s="18"/>
-    </row>
-    <row r="66" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J65" s="17"/>
+      <c r="K65" s="21"/>
+      <c r="L65" s="21"/>
+      <c r="M65" s="17"/>
+    </row>
+    <row r="66" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="32"/>
-      <c r="G66" s="32"/>
-      <c r="H66" s="32"/>
+      <c r="F66" s="31"/>
+      <c r="G66" s="31"/>
+      <c r="H66" s="31"/>
       <c r="I66" s="1"/>
-      <c r="J66" s="18"/>
-      <c r="K66" s="22"/>
-      <c r="L66" s="18"/>
-    </row>
-    <row r="67" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J66" s="17"/>
+      <c r="K66" s="21"/>
+      <c r="L66" s="21"/>
+      <c r="M66" s="17"/>
+    </row>
+    <row r="67" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="32"/>
-      <c r="G67" s="32"/>
-      <c r="H67" s="32"/>
+      <c r="F67" s="31"/>
+      <c r="G67" s="31"/>
+      <c r="H67" s="31"/>
       <c r="I67" s="1"/>
-      <c r="J67" s="18"/>
-      <c r="K67" s="22"/>
-      <c r="L67" s="18"/>
-    </row>
-    <row r="68" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J67" s="17"/>
+      <c r="K67" s="21"/>
+      <c r="L67" s="21"/>
+      <c r="M67" s="17"/>
+    </row>
+    <row r="68" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="32"/>
-      <c r="G68" s="32"/>
-      <c r="H68" s="32"/>
+      <c r="F68" s="31"/>
+      <c r="G68" s="31"/>
+      <c r="H68" s="31"/>
       <c r="I68" s="1"/>
-      <c r="J68" s="18"/>
-      <c r="K68" s="22"/>
-      <c r="L68" s="18"/>
-    </row>
-    <row r="69" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J68" s="17"/>
+      <c r="K68" s="21"/>
+      <c r="L68" s="21"/>
+      <c r="M68" s="17"/>
+    </row>
+    <row r="69" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="32"/>
-      <c r="G69" s="32"/>
-      <c r="H69" s="32"/>
+      <c r="F69" s="31"/>
+      <c r="G69" s="31"/>
+      <c r="H69" s="31"/>
       <c r="I69" s="1"/>
-      <c r="J69" s="18"/>
-      <c r="K69" s="22"/>
-      <c r="L69" s="18"/>
-    </row>
-    <row r="70" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J69" s="17"/>
+      <c r="K69" s="21"/>
+      <c r="L69" s="21"/>
+      <c r="M69" s="17"/>
+    </row>
+    <row r="70" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="32"/>
-      <c r="G70" s="32"/>
-      <c r="H70" s="32"/>
+      <c r="F70" s="31"/>
+      <c r="G70" s="31"/>
+      <c r="H70" s="31"/>
       <c r="I70" s="1"/>
-      <c r="J70" s="18"/>
-      <c r="K70" s="22"/>
-      <c r="L70" s="18"/>
-    </row>
-    <row r="71" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J70" s="17"/>
+      <c r="K70" s="21"/>
+      <c r="L70" s="21"/>
+      <c r="M70" s="17"/>
+    </row>
+    <row r="71" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
-      <c r="F71" s="32"/>
-      <c r="G71" s="32"/>
-      <c r="H71" s="32"/>
+      <c r="F71" s="31"/>
+      <c r="G71" s="31"/>
+      <c r="H71" s="31"/>
       <c r="I71" s="1"/>
-      <c r="J71" s="18"/>
-      <c r="K71" s="22"/>
-      <c r="L71" s="18"/>
-    </row>
-    <row r="72" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J71" s="17"/>
+      <c r="K71" s="21"/>
+      <c r="L71" s="21"/>
+      <c r="M71" s="17"/>
+    </row>
+    <row r="72" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="32"/>
-      <c r="G72" s="32"/>
-      <c r="H72" s="32"/>
+      <c r="F72" s="31"/>
+      <c r="G72" s="31"/>
+      <c r="H72" s="31"/>
       <c r="I72" s="1"/>
-      <c r="J72" s="18"/>
-      <c r="K72" s="22"/>
-      <c r="L72" s="18"/>
-    </row>
-    <row r="73" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J72" s="17"/>
+      <c r="K72" s="21"/>
+      <c r="L72" s="21"/>
+      <c r="M72" s="17"/>
+    </row>
+    <row r="73" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="32"/>
-      <c r="G73" s="32"/>
-      <c r="H73" s="32"/>
+      <c r="F73" s="31"/>
+      <c r="G73" s="31"/>
+      <c r="H73" s="31"/>
       <c r="I73" s="1"/>
-      <c r="J73" s="18"/>
-      <c r="K73" s="22"/>
-      <c r="L73" s="18"/>
-    </row>
-    <row r="74" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J73" s="17"/>
+      <c r="K73" s="21"/>
+      <c r="L73" s="21"/>
+      <c r="M73" s="17"/>
+    </row>
+    <row r="74" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="32"/>
-      <c r="G74" s="32"/>
-      <c r="H74" s="32"/>
+      <c r="F74" s="31"/>
+      <c r="G74" s="31"/>
+      <c r="H74" s="31"/>
       <c r="I74" s="1"/>
-      <c r="J74" s="18"/>
-      <c r="K74" s="22"/>
-      <c r="L74" s="18"/>
-    </row>
-    <row r="75" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J74" s="17"/>
+      <c r="K74" s="21"/>
+      <c r="L74" s="21"/>
+      <c r="M74" s="17"/>
+    </row>
+    <row r="75" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="32"/>
-      <c r="G75" s="32"/>
-      <c r="H75" s="32"/>
+      <c r="F75" s="31"/>
+      <c r="G75" s="31"/>
+      <c r="H75" s="31"/>
       <c r="I75" s="1"/>
-      <c r="J75" s="18"/>
-      <c r="K75" s="22"/>
-      <c r="L75" s="18"/>
-    </row>
-    <row r="76" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J75" s="17"/>
+      <c r="K75" s="21"/>
+      <c r="L75" s="21"/>
+      <c r="M75" s="17"/>
+    </row>
+    <row r="76" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
-      <c r="F76" s="32"/>
-      <c r="G76" s="32"/>
-      <c r="H76" s="32"/>
+      <c r="F76" s="31"/>
+      <c r="G76" s="31"/>
+      <c r="H76" s="31"/>
       <c r="I76" s="1"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="22"/>
-      <c r="L76" s="18"/>
-    </row>
-    <row r="77" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J76" s="17"/>
+      <c r="K76" s="21"/>
+      <c r="L76" s="21"/>
+      <c r="M76" s="17"/>
+    </row>
+    <row r="77" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="32"/>
-      <c r="G77" s="32"/>
-      <c r="H77" s="32"/>
+      <c r="F77" s="31"/>
+      <c r="G77" s="31"/>
+      <c r="H77" s="31"/>
       <c r="I77" s="1"/>
-      <c r="J77" s="18"/>
-      <c r="K77" s="22"/>
-      <c r="L77" s="18"/>
-    </row>
-    <row r="78" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J77" s="17"/>
+      <c r="K77" s="21"/>
+      <c r="L77" s="21"/>
+      <c r="M77" s="17"/>
+    </row>
+    <row r="78" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="32"/>
-      <c r="G78" s="32"/>
-      <c r="H78" s="32"/>
+      <c r="F78" s="31"/>
+      <c r="G78" s="31"/>
+      <c r="H78" s="31"/>
       <c r="I78" s="1"/>
-      <c r="J78" s="18"/>
-      <c r="K78" s="22"/>
-      <c r="L78" s="18"/>
-    </row>
-    <row r="79" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J78" s="17"/>
+      <c r="K78" s="21"/>
+      <c r="L78" s="21"/>
+      <c r="M78" s="17"/>
+    </row>
+    <row r="79" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
-      <c r="F79" s="32"/>
-      <c r="G79" s="32"/>
-      <c r="H79" s="32"/>
+      <c r="F79" s="31"/>
+      <c r="G79" s="31"/>
+      <c r="H79" s="31"/>
       <c r="I79" s="1"/>
-      <c r="J79" s="18"/>
-      <c r="K79" s="22"/>
-      <c r="L79" s="18"/>
-    </row>
-    <row r="80" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J79" s="17"/>
+      <c r="K79" s="21"/>
+      <c r="L79" s="21"/>
+      <c r="M79" s="17"/>
+    </row>
+    <row r="80" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
-      <c r="F80" s="32"/>
-      <c r="G80" s="32"/>
-      <c r="H80" s="32"/>
+      <c r="F80" s="31"/>
+      <c r="G80" s="31"/>
+      <c r="H80" s="31"/>
       <c r="I80" s="1"/>
-      <c r="J80" s="18"/>
-      <c r="K80" s="22"/>
-      <c r="L80" s="18"/>
-    </row>
-    <row r="81" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J80" s="17"/>
+      <c r="K80" s="21"/>
+      <c r="L80" s="21"/>
+      <c r="M80" s="17"/>
+    </row>
+    <row r="81" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
-      <c r="F81" s="32"/>
-      <c r="G81" s="32"/>
-      <c r="H81" s="32"/>
+      <c r="F81" s="31"/>
+      <c r="G81" s="31"/>
+      <c r="H81" s="31"/>
       <c r="I81" s="1"/>
-      <c r="J81" s="18"/>
-      <c r="K81" s="22"/>
-      <c r="L81" s="18"/>
-    </row>
-    <row r="82" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J81" s="17"/>
+      <c r="K81" s="21"/>
+      <c r="L81" s="21"/>
+      <c r="M81" s="17"/>
+    </row>
+    <row r="82" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
-      <c r="F82" s="32"/>
-      <c r="G82" s="32"/>
-      <c r="H82" s="32"/>
+      <c r="F82" s="31"/>
+      <c r="G82" s="31"/>
+      <c r="H82" s="31"/>
       <c r="I82" s="1"/>
-      <c r="J82" s="18"/>
-      <c r="K82" s="22"/>
-      <c r="L82" s="18"/>
-    </row>
-    <row r="83" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J82" s="17"/>
+      <c r="K82" s="21"/>
+      <c r="L82" s="21"/>
+      <c r="M82" s="17"/>
+    </row>
+    <row r="83" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
-      <c r="F83" s="32"/>
-      <c r="G83" s="32"/>
-      <c r="H83" s="32"/>
+      <c r="F83" s="31"/>
+      <c r="G83" s="31"/>
+      <c r="H83" s="31"/>
       <c r="I83" s="1"/>
-      <c r="J83" s="18"/>
-      <c r="K83" s="22"/>
-      <c r="L83" s="18"/>
-    </row>
-    <row r="84" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J83" s="17"/>
+      <c r="K83" s="21"/>
+      <c r="L83" s="21"/>
+      <c r="M83" s="17"/>
+    </row>
+    <row r="84" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="32"/>
-      <c r="G84" s="32"/>
-      <c r="H84" s="32"/>
+      <c r="F84" s="31"/>
+      <c r="G84" s="31"/>
+      <c r="H84" s="31"/>
       <c r="I84" s="1"/>
-      <c r="J84" s="18"/>
-      <c r="K84" s="22"/>
-      <c r="L84" s="18"/>
-    </row>
-    <row r="85" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J84" s="17"/>
+      <c r="K84" s="21"/>
+      <c r="L84" s="21"/>
+      <c r="M84" s="17"/>
+    </row>
+    <row r="85" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="32"/>
-      <c r="G85" s="32"/>
-      <c r="H85" s="32"/>
+      <c r="F85" s="31"/>
+      <c r="G85" s="31"/>
+      <c r="H85" s="31"/>
       <c r="I85" s="1"/>
-      <c r="J85" s="18"/>
-      <c r="K85" s="22"/>
-      <c r="L85" s="18"/>
-    </row>
-    <row r="86" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J85" s="17"/>
+      <c r="K85" s="21"/>
+      <c r="L85" s="21"/>
+      <c r="M85" s="17"/>
+    </row>
+    <row r="86" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
-      <c r="F86" s="32"/>
-      <c r="G86" s="32"/>
-      <c r="H86" s="32"/>
+      <c r="F86" s="31"/>
+      <c r="G86" s="31"/>
+      <c r="H86" s="31"/>
       <c r="I86" s="1"/>
-      <c r="J86" s="18"/>
-      <c r="K86" s="22"/>
-      <c r="L86" s="18"/>
-    </row>
-    <row r="87" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J86" s="17"/>
+      <c r="K86" s="21"/>
+      <c r="L86" s="21"/>
+      <c r="M86" s="17"/>
+    </row>
+    <row r="87" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
-      <c r="F87" s="32"/>
-      <c r="G87" s="32"/>
-      <c r="H87" s="32"/>
+      <c r="F87" s="31"/>
+      <c r="G87" s="31"/>
+      <c r="H87" s="31"/>
       <c r="I87" s="1"/>
-      <c r="J87" s="18"/>
-      <c r="K87" s="22"/>
-      <c r="L87" s="18"/>
-    </row>
-    <row r="88" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J87" s="17"/>
+      <c r="K87" s="21"/>
+      <c r="L87" s="21"/>
+      <c r="M87" s="17"/>
+    </row>
+    <row r="88" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
-      <c r="F88" s="32"/>
-      <c r="G88" s="32"/>
-      <c r="H88" s="32"/>
+      <c r="F88" s="31"/>
+      <c r="G88" s="31"/>
+      <c r="H88" s="31"/>
       <c r="I88" s="1"/>
-      <c r="J88" s="18"/>
-      <c r="K88" s="22"/>
-      <c r="L88" s="18"/>
-    </row>
-    <row r="89" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J88" s="17"/>
+      <c r="K88" s="21"/>
+      <c r="L88" s="21"/>
+      <c r="M88" s="17"/>
+    </row>
+    <row r="89" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
-      <c r="F89" s="32"/>
-      <c r="G89" s="32"/>
-      <c r="H89" s="32"/>
+      <c r="F89" s="31"/>
+      <c r="G89" s="31"/>
+      <c r="H89" s="31"/>
       <c r="I89" s="1"/>
-      <c r="J89" s="18"/>
-      <c r="K89" s="22"/>
-      <c r="L89" s="18"/>
-    </row>
-    <row r="90" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J89" s="17"/>
+      <c r="K89" s="21"/>
+      <c r="L89" s="21"/>
+      <c r="M89" s="17"/>
+    </row>
+    <row r="90" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
-      <c r="F90" s="32"/>
-      <c r="G90" s="32"/>
-      <c r="H90" s="32"/>
+      <c r="F90" s="31"/>
+      <c r="G90" s="31"/>
+      <c r="H90" s="31"/>
       <c r="I90" s="1"/>
-      <c r="J90" s="18"/>
-      <c r="K90" s="22"/>
-      <c r="L90" s="18"/>
-    </row>
-    <row r="91" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J90" s="17"/>
+      <c r="K90" s="21"/>
+      <c r="L90" s="21"/>
+      <c r="M90" s="17"/>
+    </row>
+    <row r="91" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
-      <c r="F91" s="32"/>
-      <c r="G91" s="32"/>
-      <c r="H91" s="32"/>
+      <c r="F91" s="31"/>
+      <c r="G91" s="31"/>
+      <c r="H91" s="31"/>
       <c r="I91" s="1"/>
-      <c r="J91" s="18"/>
-      <c r="K91" s="22"/>
-      <c r="L91" s="18"/>
-    </row>
-    <row r="92" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J91" s="17"/>
+      <c r="K91" s="21"/>
+      <c r="L91" s="21"/>
+      <c r="M91" s="17"/>
+    </row>
+    <row r="92" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
-      <c r="F92" s="32"/>
-      <c r="G92" s="32"/>
-      <c r="H92" s="32"/>
+      <c r="F92" s="31"/>
+      <c r="G92" s="31"/>
+      <c r="H92" s="31"/>
       <c r="I92" s="1"/>
-      <c r="J92" s="18"/>
-      <c r="K92" s="22"/>
-      <c r="L92" s="18"/>
-    </row>
-    <row r="93" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J92" s="17"/>
+      <c r="K92" s="21"/>
+      <c r="L92" s="21"/>
+      <c r="M92" s="17"/>
+    </row>
+    <row r="93" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
-      <c r="F93" s="32"/>
-      <c r="G93" s="32"/>
-      <c r="H93" s="32"/>
+      <c r="F93" s="31"/>
+      <c r="G93" s="31"/>
+      <c r="H93" s="31"/>
       <c r="I93" s="1"/>
-      <c r="J93" s="18"/>
-      <c r="K93" s="22"/>
-      <c r="L93" s="18"/>
-    </row>
-    <row r="94" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J93" s="17"/>
+      <c r="K93" s="21"/>
+      <c r="L93" s="21"/>
+      <c r="M93" s="17"/>
+    </row>
+    <row r="94" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
-      <c r="F94" s="32"/>
-      <c r="G94" s="32"/>
-      <c r="H94" s="32"/>
+      <c r="F94" s="31"/>
+      <c r="G94" s="31"/>
+      <c r="H94" s="31"/>
       <c r="I94" s="1"/>
-      <c r="J94" s="18"/>
-      <c r="K94" s="22"/>
-      <c r="L94" s="18"/>
-    </row>
-    <row r="95" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J94" s="17"/>
+      <c r="K94" s="21"/>
+      <c r="L94" s="21"/>
+      <c r="M94" s="17"/>
+    </row>
+    <row r="95" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
-      <c r="F95" s="32"/>
-      <c r="G95" s="32"/>
-      <c r="H95" s="32"/>
+      <c r="F95" s="31"/>
+      <c r="G95" s="31"/>
+      <c r="H95" s="31"/>
       <c r="I95" s="1"/>
-      <c r="J95" s="18"/>
-      <c r="K95" s="22"/>
-      <c r="L95" s="18"/>
-    </row>
-    <row r="96" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J95" s="17"/>
+      <c r="K95" s="21"/>
+      <c r="L95" s="21"/>
+      <c r="M95" s="17"/>
+    </row>
+    <row r="96" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
-      <c r="F96" s="32"/>
-      <c r="G96" s="32"/>
-      <c r="H96" s="32"/>
+      <c r="F96" s="31"/>
+      <c r="G96" s="31"/>
+      <c r="H96" s="31"/>
       <c r="I96" s="1"/>
-      <c r="J96" s="18"/>
-      <c r="K96" s="22"/>
-      <c r="L96" s="18"/>
-    </row>
-    <row r="97" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J96" s="17"/>
+      <c r="K96" s="21"/>
+      <c r="L96" s="21"/>
+      <c r="M96" s="17"/>
+    </row>
+    <row r="97" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
-      <c r="F97" s="32"/>
-      <c r="G97" s="32"/>
-      <c r="H97" s="32"/>
+      <c r="F97" s="31"/>
+      <c r="G97" s="31"/>
+      <c r="H97" s="31"/>
       <c r="I97" s="1"/>
-      <c r="J97" s="18"/>
-      <c r="K97" s="22"/>
-      <c r="L97" s="18"/>
-    </row>
-    <row r="98" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J97" s="17"/>
+      <c r="K97" s="21"/>
+      <c r="L97" s="21"/>
+      <c r="M97" s="17"/>
+    </row>
+    <row r="98" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
-      <c r="F98" s="32"/>
-      <c r="G98" s="32"/>
-      <c r="H98" s="32"/>
+      <c r="F98" s="31"/>
+      <c r="G98" s="31"/>
+      <c r="H98" s="31"/>
       <c r="I98" s="1"/>
-      <c r="J98" s="18"/>
-      <c r="K98" s="22"/>
-      <c r="L98" s="18"/>
-    </row>
-    <row r="99" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J98" s="17"/>
+      <c r="K98" s="21"/>
+      <c r="L98" s="21"/>
+      <c r="M98" s="17"/>
+    </row>
+    <row r="99" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
-      <c r="F99" s="32"/>
-      <c r="G99" s="32"/>
-      <c r="H99" s="32"/>
+      <c r="F99" s="31"/>
+      <c r="G99" s="31"/>
+      <c r="H99" s="31"/>
       <c r="I99" s="1"/>
-      <c r="J99" s="18"/>
-      <c r="K99" s="22"/>
-      <c r="L99" s="18"/>
-    </row>
-    <row r="100" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J99" s="17"/>
+      <c r="K99" s="21"/>
+      <c r="L99" s="21"/>
+      <c r="M99" s="17"/>
+    </row>
+    <row r="100" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
-      <c r="F100" s="32"/>
-      <c r="G100" s="32"/>
-      <c r="H100" s="32"/>
+      <c r="F100" s="31"/>
+      <c r="G100" s="31"/>
+      <c r="H100" s="31"/>
       <c r="I100" s="1"/>
-      <c r="J100" s="18"/>
-      <c r="K100" s="22"/>
-      <c r="L100" s="18"/>
-    </row>
-    <row r="101" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="J100" s="17"/>
+      <c r="K100" s="21"/>
+      <c r="L100" s="21"/>
+      <c r="M100" s="17"/>
+    </row>
+    <row r="101" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
-      <c r="F101" s="32"/>
-      <c r="G101" s="32"/>
-      <c r="H101" s="32"/>
+      <c r="F101" s="31"/>
+      <c r="G101" s="31"/>
+      <c r="H101" s="31"/>
       <c r="I101" s="1"/>
-      <c r="J101" s="18"/>
-      <c r="K101" s="22"/>
-      <c r="L101" s="18"/>
-    </row>
-    <row r="102" spans="1:12" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="4"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5"/>
-      <c r="E102" s="5"/>
-      <c r="F102" s="33"/>
-      <c r="G102" s="33"/>
-      <c r="H102" s="33"/>
-      <c r="I102" s="5"/>
-      <c r="J102" s="23"/>
-      <c r="K102" s="24"/>
-      <c r="L102" s="18"/>
-    </row>
-    <row r="103" spans="1:12" ht="30" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="K103" s="25"/>
+      <c r="J101" s="17"/>
+      <c r="K101" s="21"/>
+      <c r="L101" s="21"/>
+      <c r="M101" s="17"/>
+    </row>
+    <row r="102" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="3"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+      <c r="D102" s="1"/>
+      <c r="E102" s="1"/>
+      <c r="F102" s="31"/>
+      <c r="G102" s="31"/>
+      <c r="H102" s="31"/>
+      <c r="I102" s="1"/>
+      <c r="J102" s="17"/>
+      <c r="K102" s="21"/>
+      <c r="L102" s="21"/>
+      <c r="M102" s="17"/>
+    </row>
+    <row r="103" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A103" s="3"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+      <c r="D103" s="1"/>
+      <c r="E103" s="1"/>
+      <c r="F103" s="31"/>
+      <c r="G103" s="31"/>
+      <c r="H103" s="31"/>
+      <c r="I103" s="1"/>
+      <c r="J103" s="17"/>
+      <c r="K103" s="21"/>
+      <c r="L103" s="21"/>
+      <c r="M103" s="17"/>
+    </row>
+    <row r="104" spans="1:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A104" s="4"/>
+      <c r="B104" s="5"/>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5"/>
+      <c r="E104" s="5"/>
+      <c r="F104" s="32"/>
+      <c r="G104" s="32"/>
+      <c r="H104" s="32"/>
+      <c r="I104" s="5"/>
+      <c r="J104" s="22"/>
+      <c r="K104" s="23"/>
+      <c r="L104" s="35"/>
+      <c r="M104" s="17"/>
+    </row>
+    <row r="105" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="K105" s="24"/>
+      <c r="L105" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="20">
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="A14:L14"/>
-    <mergeCell ref="L15:L16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="E15:E16"/>
-    <mergeCell ref="F15:H15"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="I4:I5"/>
-    <mergeCell ref="F4:H4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="L4:L5"/>
+  <mergeCells count="32">
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="M16:M18"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="J16:L16"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F4:I4"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:H5"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="C17:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
english version of simple tracing importer inited
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_simple_de.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/FCL_Backtrace_Prod_simple_de.xlsx
@@ -1226,40 +1226,11 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="33" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1267,34 +1238,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="30" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="8" fillId="6" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1315,16 +1271,60 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="30" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="33" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1788,90 +1788,90 @@
     </row>
     <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:14" s="11" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="58" t="s">
+      <c r="A3" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="59"/>
-      <c r="C3" s="59"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="59"/>
-      <c r="F3" s="59"/>
-      <c r="G3" s="59"/>
-      <c r="H3" s="59"/>
-      <c r="I3" s="59"/>
-      <c r="J3" s="59"/>
-      <c r="K3" s="59"/>
-      <c r="L3" s="59"/>
-      <c r="M3" s="59"/>
+      <c r="B3" s="46"/>
+      <c r="C3" s="46"/>
+      <c r="D3" s="46"/>
+      <c r="E3" s="46"/>
+      <c r="F3" s="46"/>
+      <c r="G3" s="46"/>
+      <c r="H3" s="46"/>
+      <c r="I3" s="46"/>
+      <c r="J3" s="46"/>
+      <c r="K3" s="46"/>
+      <c r="L3" s="46"/>
+      <c r="M3" s="46"/>
     </row>
     <row r="4" spans="1:14" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="58" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="65" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="51"/>
-      <c r="D4" s="50" t="s">
+      <c r="C4" s="43"/>
+      <c r="D4" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="51"/>
-      <c r="F4" s="53" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="46" t="s">
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="47"/>
-      <c r="L4" s="47"/>
-      <c r="M4" s="43" t="s">
+      <c r="K4" s="39"/>
+      <c r="L4" s="39"/>
+      <c r="M4" s="60" t="s">
         <v>8</v>
       </c>
       <c r="N4" s="12"/>
     </row>
     <row r="5" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="39"/>
-      <c r="B5" s="46" t="s">
+      <c r="A5" s="56"/>
+      <c r="B5" s="38" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="46" t="s">
+      <c r="C5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="F5" s="55" t="s">
+      <c r="F5" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="G5" s="47"/>
-      <c r="H5" s="47"/>
-      <c r="I5" s="63" t="s">
+      <c r="G5" s="39"/>
+      <c r="H5" s="39"/>
+      <c r="I5" s="50" t="s">
         <v>31</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="K5" s="65" t="s">
+      <c r="K5" s="52" t="s">
         <v>18</v>
       </c>
-      <c r="L5" s="65" t="s">
+      <c r="L5" s="52" t="s">
         <v>27</v>
       </c>
-      <c r="M5" s="44"/>
+      <c r="M5" s="61"/>
       <c r="N5" s="12"/>
     </row>
     <row r="6" spans="1:14" ht="12.4" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="42"/>
-      <c r="B6" s="47"/>
-      <c r="C6" s="47"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
+      <c r="A6" s="59"/>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
       <c r="F6" s="28" t="s">
         <v>0</v>
       </c>
@@ -1881,11 +1881,11 @@
       <c r="H6" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="57"/>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
-      <c r="M6" s="45"/>
+      <c r="I6" s="51"/>
+      <c r="J6" s="37"/>
+      <c r="K6" s="37"/>
+      <c r="L6" s="37"/>
+      <c r="M6" s="62"/>
     </row>
     <row r="7" spans="1:14" s="11" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="13" t="s">
@@ -2011,88 +2011,88 @@
       <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="47" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="61"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="61"/>
-      <c r="J15" s="61"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="62"/>
+      <c r="B15" s="48"/>
+      <c r="C15" s="48"/>
+      <c r="D15" s="48"/>
+      <c r="E15" s="48"/>
+      <c r="F15" s="48"/>
+      <c r="G15" s="48"/>
+      <c r="H15" s="48"/>
+      <c r="I15" s="48"/>
+      <c r="J15" s="48"/>
+      <c r="K15" s="48"/>
+      <c r="L15" s="48"/>
+      <c r="M15" s="49"/>
     </row>
     <row r="16" spans="1:14" s="20" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="39" t="s">
+      <c r="A16" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="66" t="s">
         <v>26</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52" t="s">
+      <c r="C16" s="43"/>
+      <c r="D16" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="67" t="s">
+      <c r="E16" s="43"/>
+      <c r="F16" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="51"/>
-      <c r="J16" s="48" t="s">
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="49"/>
-      <c r="L16" s="47"/>
-      <c r="M16" s="36" t="s">
+      <c r="K16" s="64"/>
+      <c r="L16" s="39"/>
+      <c r="M16" s="53" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:13" s="20" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="39"/>
-      <c r="B17" s="56" t="s">
+      <c r="A17" s="56"/>
+      <c r="B17" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C17" s="56" t="s">
+      <c r="C17" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="D17" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="56" t="s">
+      <c r="E17" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="F17" s="67" t="s">
+      <c r="F17" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="68"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="56" t="s">
+      <c r="G17" s="42"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="J17" s="66" t="s">
+      <c r="J17" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="K17" s="66" t="s">
+      <c r="K17" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="L17" s="66" t="s">
+      <c r="L17" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="M17" s="37"/>
+      <c r="M17" s="54"/>
     </row>
     <row r="18" spans="1:13" s="20" customFormat="1" ht="23.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="40"/>
-      <c r="B18" s="57"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
+      <c r="A18" s="57"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="33" t="s">
         <v>0</v>
       </c>
@@ -2102,11 +2102,11 @@
       <c r="H18" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="38"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="37"/>
+      <c r="K18" s="37"/>
+      <c r="L18" s="37"/>
+      <c r="M18" s="55"/>
     </row>
     <row r="19" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
@@ -3404,22 +3404,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="J17:J18"/>
-    <mergeCell ref="K17:K18"/>
-    <mergeCell ref="L17:L18"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E17:E18"/>
-    <mergeCell ref="F17:H17"/>
-    <mergeCell ref="I17:I18"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="A3:M3"/>
-    <mergeCell ref="A15:M15"/>
-    <mergeCell ref="I5:I6"/>
-    <mergeCell ref="J5:J6"/>
-    <mergeCell ref="K5:K6"/>
-    <mergeCell ref="L5:L6"/>
     <mergeCell ref="M16:M18"/>
     <mergeCell ref="A16:A18"/>
     <mergeCell ref="A4:A6"/>
@@ -3436,7 +3420,37 @@
     <mergeCell ref="F5:H5"/>
     <mergeCell ref="B17:B18"/>
     <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A3:M3"/>
+    <mergeCell ref="A15:M15"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="J5:J6"/>
+    <mergeCell ref="K5:K6"/>
+    <mergeCell ref="L5:L6"/>
+    <mergeCell ref="J17:J18"/>
+    <mergeCell ref="K17:K18"/>
+    <mergeCell ref="L17:L18"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="F17:H17"/>
+    <mergeCell ref="I17:I18"/>
+    <mergeCell ref="F16:I16"/>
   </mergeCells>
+  <dataValidations count="3">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1:F1048576">
+      <formula1>1</formula1>
+      <formula2>31</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G1:G1048576">
+      <formula1>1</formula1>
+      <formula2>12</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H1:H1048576">
+      <formula1>1900</formula1>
+      <formula2>2100</formula2>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>